<commit_message>
XML-feat: thread models DFDs updated
</commit_message>
<xml_diff>
--- a/settings-microservice.xlsx
+++ b/settings-microservice.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F37C3EE-C318-4459-9132-4B1F01A8E89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740CB476-0075-4E41-BC47-E3FE285041BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1281,6 +1281,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1293,62 +1314,47 @@
     <xf numFmtId="49" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1364,12 +1370,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1394,14 +1394,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>136457</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>160732</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>70961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>282642</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19555</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109326</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1429,8 +1429,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2203382" y="541732"/>
-          <a:ext cx="3803785" cy="2906823"/>
+          <a:off x="2203382" y="642461"/>
+          <a:ext cx="3803785" cy="2705365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1443,14 +1443,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>25533</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>79834</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>177993</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>407818</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>148455</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>50296</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1478,8 +1478,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1482858" y="4080334"/>
-          <a:ext cx="5259085" cy="4259621"/>
+          <a:off x="1482858" y="4368993"/>
+          <a:ext cx="5259085" cy="3682303"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1492,14 +1492,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>409112</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>29623</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>13575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>429090</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>108328</xdr:rowOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>124375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1527,8 +1527,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1866437" y="8602123"/>
-          <a:ext cx="4896778" cy="5412705"/>
+          <a:off x="1866437" y="8776575"/>
+          <a:ext cx="4896778" cy="5063800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1541,10 +1541,10 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>602945</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>29623</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>115877</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4509111" cy="5412705"/>
+    <xdr:ext cx="4509111" cy="4859197"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Picture 4">
@@ -1571,8 +1571,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2060270" y="14317123"/>
-          <a:ext cx="4509111" cy="5412705"/>
+          <a:off x="2060270" y="14593877"/>
+          <a:ext cx="4509111" cy="4859197"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1584,11 +1584,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>455722</xdr:colOff>
+      <xdr:colOff>463420</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>29623</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4803558" cy="5412705"/>
+    <xdr:ext cx="4788162" cy="5412705"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="Picture 6">
@@ -1615,8 +1615,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1913047" y="20032123"/>
-          <a:ext cx="4803558" cy="5412705"/>
+          <a:off x="1920745" y="20032123"/>
+          <a:ext cx="4788162" cy="5412705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2042,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,11 +2055,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2080,10 +2080,10 @@
       <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="62"/>
+      <c r="C3" s="69"/>
       <c r="D3" s="35"/>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2202,10 +2202,10 @@
       <c r="A12" s="15">
         <v>2</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="60"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2318,10 +2318,10 @@
       <c r="A21" s="15">
         <v>3</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="60"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="35"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2391,11 +2391,11 @@
       <c r="D26" s="34"/>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
       <c r="D27" s="24"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2553,99 +2553,99 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="65"/>
+      <c r="C40" s="61"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>1</v>
       </c>
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="69"/>
+      <c r="C41" s="64"/>
     </row>
     <row r="42" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="70"/>
+      <c r="C42" s="65"/>
     </row>
     <row r="43" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="70" t="s">
+      <c r="B43" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="70"/>
+      <c r="C43" s="65"/>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>2</v>
       </c>
-      <c r="B44" s="69" t="s">
+      <c r="B44" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="69"/>
+      <c r="C44" s="64"/>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="67" t="s">
+      <c r="B45" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="C45" s="68"/>
+      <c r="C45" s="63"/>
     </row>
     <row r="46" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="67" t="s">
+      <c r="B46" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="C46" s="68"/>
+      <c r="C46" s="63"/>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="67" t="s">
+      <c r="B47" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="68"/>
+      <c r="C47" s="63"/>
     </row>
     <row r="48" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="67" t="s">
+      <c r="B48" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="C48" s="68"/>
+      <c r="C48" s="63"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="B49" s="66"/>
-      <c r="C49" s="66"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
@@ -2693,6 +2693,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A27:C27"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="B40:C40"/>
@@ -2704,11 +2709,6 @@
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2719,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:O134"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="P114" sqref="P114"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="S113" sqref="S113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,289 +2747,289 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="72"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="72"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="72"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="71" t="s">
@@ -3049,349 +3049,349 @@
       <c r="N21" s="71"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="73"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="75"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="74"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="76"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="78"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="77"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="76"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77"/>
-      <c r="N24" s="78"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
+      <c r="N24" s="77"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="76"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77"/>
-      <c r="N25" s="78"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="77"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="76"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="78"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="77"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="76"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="77"/>
-      <c r="N27" s="78"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="77"/>
     </row>
     <row r="28" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="76"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="77"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="77"/>
-      <c r="J28" s="77"/>
-      <c r="K28" s="77"/>
-      <c r="L28" s="77"/>
-      <c r="M28" s="77"/>
-      <c r="N28" s="78"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="77"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="76"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="77"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="77"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="77"/>
-      <c r="N29" s="78"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="76"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="76"/>
+      <c r="N29" s="77"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="76"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="77"/>
-      <c r="N30" s="78"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="76"/>
+      <c r="N30" s="77"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="76"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="77"/>
-      <c r="N31" s="78"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="76"/>
+      <c r="K31" s="76"/>
+      <c r="L31" s="76"/>
+      <c r="M31" s="76"/>
+      <c r="N31" s="77"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="76"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="77"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="78"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="76"/>
+      <c r="L32" s="76"/>
+      <c r="M32" s="76"/>
+      <c r="N32" s="77"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="76"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="78"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="76"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="76"/>
+      <c r="L33" s="76"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="77"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="76"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-      <c r="N34" s="78"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="77"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="76"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="77"/>
-      <c r="L35" s="77"/>
-      <c r="M35" s="77"/>
-      <c r="N35" s="78"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="76"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="76"/>
+      <c r="N35" s="77"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="76"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="77"/>
-      <c r="L36" s="77"/>
-      <c r="M36" s="77"/>
-      <c r="N36" s="78"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="77"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="76"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="77"/>
-      <c r="L37" s="77"/>
-      <c r="M37" s="77"/>
-      <c r="N37" s="78"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="77"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="76"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="77"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="77"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="78"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="76"/>
+      <c r="N38" s="77"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="76"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="77"/>
-      <c r="J39" s="77"/>
-      <c r="K39" s="77"/>
-      <c r="L39" s="77"/>
-      <c r="M39" s="77"/>
-      <c r="N39" s="78"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="76"/>
+      <c r="M39" s="76"/>
+      <c r="N39" s="77"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="76"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="77"/>
-      <c r="J40" s="77"/>
-      <c r="K40" s="77"/>
-      <c r="L40" s="77"/>
-      <c r="M40" s="77"/>
-      <c r="N40" s="78"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="76"/>
+      <c r="J40" s="76"/>
+      <c r="K40" s="76"/>
+      <c r="L40" s="76"/>
+      <c r="M40" s="76"/>
+      <c r="N40" s="77"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="76"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="77"/>
-      <c r="K41" s="77"/>
-      <c r="L41" s="77"/>
-      <c r="M41" s="77"/>
-      <c r="N41" s="78"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="76"/>
+      <c r="N41" s="77"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="76"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77"/>
-      <c r="J42" s="77"/>
-      <c r="K42" s="77"/>
-      <c r="L42" s="77"/>
-      <c r="M42" s="77"/>
-      <c r="N42" s="78"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
+      <c r="N42" s="77"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="76"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="77"/>
-      <c r="G43" s="77"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="77"/>
-      <c r="L43" s="77"/>
-      <c r="M43" s="77"/>
-      <c r="N43" s="78"/>
+      <c r="B43" s="75"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="77"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="79"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="80"/>
-      <c r="J44" s="80"/>
-      <c r="K44" s="80"/>
-      <c r="L44" s="80"/>
-      <c r="M44" s="80"/>
-      <c r="N44" s="81"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="79"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="79"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="79"/>
+      <c r="N44" s="80"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="71" t="s">
@@ -3411,439 +3411,439 @@
       <c r="N45" s="71"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="73"/>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="74"/>
-      <c r="M46" s="74"/>
-      <c r="N46" s="75"/>
+      <c r="B46" s="72"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="73"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="73"/>
+      <c r="M46" s="73"/>
+      <c r="N46" s="74"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="76"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="77"/>
-      <c r="J47" s="77"/>
-      <c r="K47" s="77"/>
-      <c r="L47" s="77"/>
-      <c r="M47" s="77"/>
-      <c r="N47" s="78"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="77"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="76"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="77"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="77"/>
-      <c r="I48" s="77"/>
-      <c r="J48" s="77"/>
-      <c r="K48" s="77"/>
-      <c r="L48" s="77"/>
-      <c r="M48" s="77"/>
-      <c r="N48" s="78"/>
+      <c r="B48" s="75"/>
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="76"/>
+      <c r="G48" s="76"/>
+      <c r="H48" s="76"/>
+      <c r="I48" s="76"/>
+      <c r="J48" s="76"/>
+      <c r="K48" s="76"/>
+      <c r="L48" s="76"/>
+      <c r="M48" s="76"/>
+      <c r="N48" s="77"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="76"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="77"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="77"/>
-      <c r="I49" s="77"/>
-      <c r="J49" s="77"/>
-      <c r="K49" s="77"/>
-      <c r="L49" s="77"/>
-      <c r="M49" s="77"/>
-      <c r="N49" s="78"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="76"/>
+      <c r="M49" s="76"/>
+      <c r="N49" s="77"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="76"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="77"/>
-      <c r="F50" s="77"/>
-      <c r="G50" s="77"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="77"/>
-      <c r="J50" s="77"/>
-      <c r="K50" s="77"/>
-      <c r="L50" s="77"/>
-      <c r="M50" s="77"/>
-      <c r="N50" s="78"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="76"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="76"/>
+      <c r="L50" s="76"/>
+      <c r="M50" s="76"/>
+      <c r="N50" s="77"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="76"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="77"/>
-      <c r="J51" s="77"/>
-      <c r="K51" s="77"/>
-      <c r="L51" s="77"/>
-      <c r="M51" s="77"/>
-      <c r="N51" s="78"/>
+      <c r="B51" s="75"/>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="76"/>
+      <c r="M51" s="76"/>
+      <c r="N51" s="77"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="76"/>
-      <c r="C52" s="77"/>
-      <c r="D52" s="77"/>
-      <c r="E52" s="77"/>
-      <c r="F52" s="77"/>
-      <c r="G52" s="77"/>
-      <c r="H52" s="77"/>
-      <c r="I52" s="77"/>
-      <c r="J52" s="77"/>
-      <c r="K52" s="77"/>
-      <c r="L52" s="77"/>
-      <c r="M52" s="77"/>
-      <c r="N52" s="78"/>
+      <c r="B52" s="75"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="76"/>
+      <c r="M52" s="76"/>
+      <c r="N52" s="77"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="76"/>
-      <c r="C53" s="77"/>
-      <c r="D53" s="77"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="77"/>
-      <c r="G53" s="77"/>
-      <c r="H53" s="77"/>
-      <c r="I53" s="77"/>
-      <c r="J53" s="77"/>
-      <c r="K53" s="77"/>
-      <c r="L53" s="77"/>
-      <c r="M53" s="77"/>
-      <c r="N53" s="78"/>
+      <c r="B53" s="75"/>
+      <c r="C53" s="76"/>
+      <c r="D53" s="76"/>
+      <c r="E53" s="76"/>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="76"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="77"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="76"/>
-      <c r="C54" s="77"/>
-      <c r="D54" s="77"/>
-      <c r="E54" s="77"/>
-      <c r="F54" s="77"/>
-      <c r="G54" s="77"/>
-      <c r="H54" s="77"/>
-      <c r="I54" s="77"/>
-      <c r="J54" s="77"/>
-      <c r="K54" s="77"/>
-      <c r="L54" s="77"/>
-      <c r="M54" s="77"/>
-      <c r="N54" s="78"/>
+      <c r="B54" s="75"/>
+      <c r="C54" s="76"/>
+      <c r="D54" s="76"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="76"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="76"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="76"/>
+      <c r="M54" s="76"/>
+      <c r="N54" s="77"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="76"/>
-      <c r="C55" s="77"/>
-      <c r="D55" s="77"/>
-      <c r="E55" s="77"/>
-      <c r="F55" s="77"/>
-      <c r="G55" s="77"/>
-      <c r="H55" s="77"/>
-      <c r="I55" s="77"/>
-      <c r="J55" s="77"/>
-      <c r="K55" s="77"/>
-      <c r="L55" s="77"/>
-      <c r="M55" s="77"/>
-      <c r="N55" s="78"/>
+      <c r="B55" s="75"/>
+      <c r="C55" s="76"/>
+      <c r="D55" s="76"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="76"/>
+      <c r="G55" s="76"/>
+      <c r="H55" s="76"/>
+      <c r="I55" s="76"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="76"/>
+      <c r="M55" s="76"/>
+      <c r="N55" s="77"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="76"/>
-      <c r="C56" s="77"/>
-      <c r="D56" s="77"/>
-      <c r="E56" s="77"/>
-      <c r="F56" s="77"/>
-      <c r="G56" s="77"/>
-      <c r="H56" s="77"/>
-      <c r="I56" s="77"/>
-      <c r="J56" s="77"/>
-      <c r="K56" s="77"/>
-      <c r="L56" s="77"/>
-      <c r="M56" s="77"/>
-      <c r="N56" s="78"/>
+      <c r="B56" s="75"/>
+      <c r="C56" s="76"/>
+      <c r="D56" s="76"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="76"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="76"/>
+      <c r="M56" s="76"/>
+      <c r="N56" s="77"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="76"/>
-      <c r="C57" s="77"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="77"/>
-      <c r="F57" s="77"/>
-      <c r="G57" s="77"/>
-      <c r="H57" s="77"/>
-      <c r="I57" s="77"/>
-      <c r="J57" s="77"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="77"/>
-      <c r="M57" s="77"/>
-      <c r="N57" s="78"/>
+      <c r="B57" s="75"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="77"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="76"/>
-      <c r="C58" s="77"/>
-      <c r="D58" s="77"/>
-      <c r="E58" s="77"/>
-      <c r="F58" s="77"/>
-      <c r="G58" s="77"/>
-      <c r="H58" s="77"/>
-      <c r="I58" s="77"/>
-      <c r="J58" s="77"/>
-      <c r="K58" s="77"/>
-      <c r="L58" s="77"/>
-      <c r="M58" s="77"/>
-      <c r="N58" s="78"/>
+      <c r="B58" s="75"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="76"/>
+      <c r="G58" s="76"/>
+      <c r="H58" s="76"/>
+      <c r="I58" s="76"/>
+      <c r="J58" s="76"/>
+      <c r="K58" s="76"/>
+      <c r="L58" s="76"/>
+      <c r="M58" s="76"/>
+      <c r="N58" s="77"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="76"/>
-      <c r="C59" s="77"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="77"/>
-      <c r="F59" s="77"/>
-      <c r="G59" s="77"/>
-      <c r="H59" s="77"/>
-      <c r="I59" s="77"/>
-      <c r="J59" s="77"/>
-      <c r="K59" s="77"/>
-      <c r="L59" s="77"/>
-      <c r="M59" s="77"/>
-      <c r="N59" s="78"/>
+      <c r="B59" s="75"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="76"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="76"/>
+      <c r="L59" s="76"/>
+      <c r="M59" s="76"/>
+      <c r="N59" s="77"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="76"/>
-      <c r="C60" s="77"/>
-      <c r="D60" s="77"/>
-      <c r="E60" s="77"/>
-      <c r="F60" s="77"/>
-      <c r="G60" s="77"/>
-      <c r="H60" s="77"/>
-      <c r="I60" s="77"/>
-      <c r="J60" s="77"/>
-      <c r="K60" s="77"/>
-      <c r="L60" s="77"/>
-      <c r="M60" s="77"/>
-      <c r="N60" s="78"/>
+      <c r="B60" s="75"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="76"/>
+      <c r="M60" s="76"/>
+      <c r="N60" s="77"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="76"/>
-      <c r="C61" s="77"/>
-      <c r="D61" s="77"/>
-      <c r="E61" s="77"/>
-      <c r="F61" s="77"/>
-      <c r="G61" s="77"/>
-      <c r="H61" s="77"/>
-      <c r="I61" s="77"/>
-      <c r="J61" s="77"/>
-      <c r="K61" s="77"/>
-      <c r="L61" s="77"/>
-      <c r="M61" s="77"/>
-      <c r="N61" s="78"/>
+      <c r="B61" s="75"/>
+      <c r="C61" s="76"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="76"/>
+      <c r="G61" s="76"/>
+      <c r="H61" s="76"/>
+      <c r="I61" s="76"/>
+      <c r="J61" s="76"/>
+      <c r="K61" s="76"/>
+      <c r="L61" s="76"/>
+      <c r="M61" s="76"/>
+      <c r="N61" s="77"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="76"/>
-      <c r="C62" s="77"/>
-      <c r="D62" s="77"/>
-      <c r="E62" s="77"/>
-      <c r="F62" s="77"/>
-      <c r="G62" s="77"/>
-      <c r="H62" s="77"/>
-      <c r="I62" s="77"/>
-      <c r="J62" s="77"/>
-      <c r="K62" s="77"/>
-      <c r="L62" s="77"/>
-      <c r="M62" s="77"/>
-      <c r="N62" s="78"/>
+      <c r="B62" s="75"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="76"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="76"/>
+      <c r="G62" s="76"/>
+      <c r="H62" s="76"/>
+      <c r="I62" s="76"/>
+      <c r="J62" s="76"/>
+      <c r="K62" s="76"/>
+      <c r="L62" s="76"/>
+      <c r="M62" s="76"/>
+      <c r="N62" s="77"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="76"/>
-      <c r="C63" s="77"/>
-      <c r="D63" s="77"/>
-      <c r="E63" s="77"/>
-      <c r="F63" s="77"/>
-      <c r="G63" s="77"/>
-      <c r="H63" s="77"/>
-      <c r="I63" s="77"/>
-      <c r="J63" s="77"/>
-      <c r="K63" s="77"/>
-      <c r="L63" s="77"/>
-      <c r="M63" s="77"/>
-      <c r="N63" s="78"/>
+      <c r="B63" s="75"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="76"/>
+      <c r="J63" s="76"/>
+      <c r="K63" s="76"/>
+      <c r="L63" s="76"/>
+      <c r="M63" s="76"/>
+      <c r="N63" s="77"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="76"/>
-      <c r="C64" s="77"/>
-      <c r="D64" s="77"/>
-      <c r="E64" s="77"/>
-      <c r="F64" s="77"/>
-      <c r="G64" s="77"/>
-      <c r="H64" s="77"/>
-      <c r="I64" s="77"/>
-      <c r="J64" s="77"/>
-      <c r="K64" s="77"/>
-      <c r="L64" s="77"/>
-      <c r="M64" s="77"/>
-      <c r="N64" s="78"/>
+      <c r="B64" s="75"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="76"/>
+      <c r="G64" s="76"/>
+      <c r="H64" s="76"/>
+      <c r="I64" s="76"/>
+      <c r="J64" s="76"/>
+      <c r="K64" s="76"/>
+      <c r="L64" s="76"/>
+      <c r="M64" s="76"/>
+      <c r="N64" s="77"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B65" s="76"/>
-      <c r="C65" s="77"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="77"/>
-      <c r="F65" s="77"/>
-      <c r="G65" s="77"/>
-      <c r="H65" s="77"/>
-      <c r="I65" s="77"/>
-      <c r="J65" s="77"/>
-      <c r="K65" s="77"/>
-      <c r="L65" s="77"/>
-      <c r="M65" s="77"/>
-      <c r="N65" s="78"/>
+      <c r="B65" s="75"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="76"/>
+      <c r="G65" s="76"/>
+      <c r="H65" s="76"/>
+      <c r="I65" s="76"/>
+      <c r="J65" s="76"/>
+      <c r="K65" s="76"/>
+      <c r="L65" s="76"/>
+      <c r="M65" s="76"/>
+      <c r="N65" s="77"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B66" s="76"/>
-      <c r="C66" s="77"/>
-      <c r="D66" s="77"/>
-      <c r="E66" s="77"/>
-      <c r="F66" s="77"/>
-      <c r="G66" s="77"/>
-      <c r="H66" s="77"/>
-      <c r="I66" s="77"/>
-      <c r="J66" s="77"/>
-      <c r="K66" s="77"/>
-      <c r="L66" s="77"/>
-      <c r="M66" s="77"/>
-      <c r="N66" s="78"/>
+      <c r="B66" s="75"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="76"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="76"/>
+      <c r="I66" s="76"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="76"/>
+      <c r="L66" s="76"/>
+      <c r="M66" s="76"/>
+      <c r="N66" s="77"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="76"/>
-      <c r="C67" s="77"/>
-      <c r="D67" s="77"/>
-      <c r="E67" s="77"/>
-      <c r="F67" s="77"/>
-      <c r="G67" s="77"/>
-      <c r="H67" s="77"/>
-      <c r="I67" s="77"/>
-      <c r="J67" s="77"/>
-      <c r="K67" s="77"/>
-      <c r="L67" s="77"/>
-      <c r="M67" s="77"/>
-      <c r="N67" s="78"/>
+      <c r="B67" s="75"/>
+      <c r="C67" s="76"/>
+      <c r="D67" s="76"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="76"/>
+      <c r="G67" s="76"/>
+      <c r="H67" s="76"/>
+      <c r="I67" s="76"/>
+      <c r="J67" s="76"/>
+      <c r="K67" s="76"/>
+      <c r="L67" s="76"/>
+      <c r="M67" s="76"/>
+      <c r="N67" s="77"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="76"/>
-      <c r="C68" s="77"/>
-      <c r="D68" s="77"/>
-      <c r="E68" s="77"/>
-      <c r="F68" s="77"/>
-      <c r="G68" s="77"/>
-      <c r="H68" s="77"/>
-      <c r="I68" s="77"/>
-      <c r="J68" s="77"/>
-      <c r="K68" s="77"/>
-      <c r="L68" s="77"/>
-      <c r="M68" s="77"/>
-      <c r="N68" s="78"/>
+      <c r="B68" s="75"/>
+      <c r="C68" s="76"/>
+      <c r="D68" s="76"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="76"/>
+      <c r="G68" s="76"/>
+      <c r="H68" s="76"/>
+      <c r="I68" s="76"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="76"/>
+      <c r="L68" s="76"/>
+      <c r="M68" s="76"/>
+      <c r="N68" s="77"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="76"/>
-      <c r="C69" s="77"/>
-      <c r="D69" s="77"/>
-      <c r="E69" s="77"/>
-      <c r="F69" s="77"/>
-      <c r="G69" s="77"/>
-      <c r="H69" s="77"/>
-      <c r="I69" s="77"/>
-      <c r="J69" s="77"/>
-      <c r="K69" s="77"/>
-      <c r="L69" s="77"/>
-      <c r="M69" s="77"/>
-      <c r="N69" s="78"/>
+      <c r="B69" s="75"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="76"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="76"/>
+      <c r="L69" s="76"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="77"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B70" s="76"/>
-      <c r="C70" s="77"/>
-      <c r="D70" s="77"/>
-      <c r="E70" s="77"/>
-      <c r="F70" s="77"/>
-      <c r="G70" s="77"/>
-      <c r="H70" s="77"/>
-      <c r="I70" s="77"/>
-      <c r="J70" s="77"/>
-      <c r="K70" s="77"/>
-      <c r="L70" s="77"/>
-      <c r="M70" s="77"/>
-      <c r="N70" s="78"/>
+      <c r="B70" s="75"/>
+      <c r="C70" s="76"/>
+      <c r="D70" s="76"/>
+      <c r="E70" s="76"/>
+      <c r="F70" s="76"/>
+      <c r="G70" s="76"/>
+      <c r="H70" s="76"/>
+      <c r="I70" s="76"/>
+      <c r="J70" s="76"/>
+      <c r="K70" s="76"/>
+      <c r="L70" s="76"/>
+      <c r="M70" s="76"/>
+      <c r="N70" s="77"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B71" s="76"/>
-      <c r="C71" s="77"/>
-      <c r="D71" s="77"/>
-      <c r="E71" s="77"/>
-      <c r="F71" s="77"/>
-      <c r="G71" s="77"/>
-      <c r="H71" s="77"/>
-      <c r="I71" s="77"/>
-      <c r="J71" s="77"/>
-      <c r="K71" s="77"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="77"/>
-      <c r="N71" s="78"/>
+      <c r="B71" s="75"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="76"/>
+      <c r="E71" s="76"/>
+      <c r="F71" s="76"/>
+      <c r="G71" s="76"/>
+      <c r="H71" s="76"/>
+      <c r="I71" s="76"/>
+      <c r="J71" s="76"/>
+      <c r="K71" s="76"/>
+      <c r="L71" s="76"/>
+      <c r="M71" s="76"/>
+      <c r="N71" s="77"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B72" s="76"/>
-      <c r="C72" s="77"/>
-      <c r="D72" s="77"/>
-      <c r="E72" s="77"/>
-      <c r="F72" s="77"/>
-      <c r="G72" s="77"/>
-      <c r="H72" s="77"/>
-      <c r="I72" s="77"/>
-      <c r="J72" s="77"/>
-      <c r="K72" s="77"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="77"/>
-      <c r="N72" s="78"/>
+      <c r="B72" s="75"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
+      <c r="H72" s="76"/>
+      <c r="I72" s="76"/>
+      <c r="J72" s="76"/>
+      <c r="K72" s="76"/>
+      <c r="L72" s="76"/>
+      <c r="M72" s="76"/>
+      <c r="N72" s="77"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="76"/>
-      <c r="C73" s="77"/>
-      <c r="D73" s="77"/>
-      <c r="E73" s="77"/>
-      <c r="F73" s="77"/>
-      <c r="G73" s="77"/>
-      <c r="H73" s="77"/>
-      <c r="I73" s="77"/>
-      <c r="J73" s="77"/>
-      <c r="K73" s="77"/>
-      <c r="L73" s="77"/>
-      <c r="M73" s="77"/>
-      <c r="N73" s="78"/>
+      <c r="B73" s="75"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="76"/>
+      <c r="J73" s="76"/>
+      <c r="K73" s="76"/>
+      <c r="L73" s="76"/>
+      <c r="M73" s="76"/>
+      <c r="N73" s="77"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="79"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="80"/>
-      <c r="E74" s="80"/>
-      <c r="F74" s="80"/>
-      <c r="G74" s="80"/>
-      <c r="H74" s="80"/>
-      <c r="I74" s="80"/>
-      <c r="J74" s="80"/>
-      <c r="K74" s="80"/>
-      <c r="L74" s="80"/>
-      <c r="M74" s="80"/>
-      <c r="N74" s="81"/>
+      <c r="B74" s="78"/>
+      <c r="C74" s="79"/>
+      <c r="D74" s="79"/>
+      <c r="E74" s="79"/>
+      <c r="F74" s="79"/>
+      <c r="G74" s="79"/>
+      <c r="H74" s="79"/>
+      <c r="I74" s="79"/>
+      <c r="J74" s="79"/>
+      <c r="K74" s="79"/>
+      <c r="L74" s="79"/>
+      <c r="M74" s="79"/>
+      <c r="N74" s="80"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" s="71" t="s">
@@ -3863,439 +3863,439 @@
       <c r="N75" s="71"/>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="73"/>
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="74"/>
-      <c r="H76" s="74"/>
-      <c r="I76" s="74"/>
-      <c r="J76" s="74"/>
-      <c r="K76" s="74"/>
-      <c r="L76" s="74"/>
-      <c r="M76" s="74"/>
-      <c r="N76" s="75"/>
+      <c r="B76" s="72"/>
+      <c r="C76" s="73"/>
+      <c r="D76" s="73"/>
+      <c r="E76" s="73"/>
+      <c r="F76" s="73"/>
+      <c r="G76" s="73"/>
+      <c r="H76" s="73"/>
+      <c r="I76" s="73"/>
+      <c r="J76" s="73"/>
+      <c r="K76" s="73"/>
+      <c r="L76" s="73"/>
+      <c r="M76" s="73"/>
+      <c r="N76" s="74"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="76"/>
-      <c r="C77" s="77"/>
-      <c r="D77" s="77"/>
-      <c r="E77" s="77"/>
-      <c r="F77" s="77"/>
-      <c r="G77" s="77"/>
-      <c r="H77" s="77"/>
-      <c r="I77" s="77"/>
-      <c r="J77" s="77"/>
-      <c r="K77" s="77"/>
-      <c r="L77" s="77"/>
-      <c r="M77" s="77"/>
-      <c r="N77" s="78"/>
+      <c r="B77" s="75"/>
+      <c r="C77" s="76"/>
+      <c r="D77" s="76"/>
+      <c r="E77" s="76"/>
+      <c r="F77" s="76"/>
+      <c r="G77" s="76"/>
+      <c r="H77" s="76"/>
+      <c r="I77" s="76"/>
+      <c r="J77" s="76"/>
+      <c r="K77" s="76"/>
+      <c r="L77" s="76"/>
+      <c r="M77" s="76"/>
+      <c r="N77" s="77"/>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B78" s="76"/>
-      <c r="C78" s="77"/>
-      <c r="D78" s="77"/>
-      <c r="E78" s="77"/>
-      <c r="F78" s="77"/>
-      <c r="G78" s="77"/>
-      <c r="H78" s="77"/>
-      <c r="I78" s="77"/>
-      <c r="J78" s="77"/>
-      <c r="K78" s="77"/>
-      <c r="L78" s="77"/>
-      <c r="M78" s="77"/>
-      <c r="N78" s="78"/>
+      <c r="B78" s="75"/>
+      <c r="C78" s="76"/>
+      <c r="D78" s="76"/>
+      <c r="E78" s="76"/>
+      <c r="F78" s="76"/>
+      <c r="G78" s="76"/>
+      <c r="H78" s="76"/>
+      <c r="I78" s="76"/>
+      <c r="J78" s="76"/>
+      <c r="K78" s="76"/>
+      <c r="L78" s="76"/>
+      <c r="M78" s="76"/>
+      <c r="N78" s="77"/>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B79" s="76"/>
-      <c r="C79" s="77"/>
-      <c r="D79" s="77"/>
-      <c r="E79" s="77"/>
-      <c r="F79" s="77"/>
-      <c r="G79" s="77"/>
-      <c r="H79" s="77"/>
-      <c r="I79" s="77"/>
-      <c r="J79" s="77"/>
-      <c r="K79" s="77"/>
-      <c r="L79" s="77"/>
-      <c r="M79" s="77"/>
-      <c r="N79" s="78"/>
+      <c r="B79" s="75"/>
+      <c r="C79" s="76"/>
+      <c r="D79" s="76"/>
+      <c r="E79" s="76"/>
+      <c r="F79" s="76"/>
+      <c r="G79" s="76"/>
+      <c r="H79" s="76"/>
+      <c r="I79" s="76"/>
+      <c r="J79" s="76"/>
+      <c r="K79" s="76"/>
+      <c r="L79" s="76"/>
+      <c r="M79" s="76"/>
+      <c r="N79" s="77"/>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B80" s="76"/>
-      <c r="C80" s="77"/>
-      <c r="D80" s="77"/>
-      <c r="E80" s="77"/>
-      <c r="F80" s="77"/>
-      <c r="G80" s="77"/>
-      <c r="H80" s="77"/>
-      <c r="I80" s="77"/>
-      <c r="J80" s="77"/>
-      <c r="K80" s="77"/>
-      <c r="L80" s="77"/>
-      <c r="M80" s="77"/>
-      <c r="N80" s="78"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="76"/>
+      <c r="D80" s="76"/>
+      <c r="E80" s="76"/>
+      <c r="F80" s="76"/>
+      <c r="G80" s="76"/>
+      <c r="H80" s="76"/>
+      <c r="I80" s="76"/>
+      <c r="J80" s="76"/>
+      <c r="K80" s="76"/>
+      <c r="L80" s="76"/>
+      <c r="M80" s="76"/>
+      <c r="N80" s="77"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="76"/>
-      <c r="C81" s="77"/>
-      <c r="D81" s="77"/>
-      <c r="E81" s="77"/>
-      <c r="F81" s="77"/>
-      <c r="G81" s="77"/>
-      <c r="H81" s="77"/>
-      <c r="I81" s="77"/>
-      <c r="J81" s="77"/>
-      <c r="K81" s="77"/>
-      <c r="L81" s="77"/>
-      <c r="M81" s="77"/>
-      <c r="N81" s="78"/>
+      <c r="B81" s="75"/>
+      <c r="C81" s="76"/>
+      <c r="D81" s="76"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="76"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
+      <c r="J81" s="76"/>
+      <c r="K81" s="76"/>
+      <c r="L81" s="76"/>
+      <c r="M81" s="76"/>
+      <c r="N81" s="77"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B82" s="76"/>
-      <c r="C82" s="77"/>
-      <c r="D82" s="77"/>
-      <c r="E82" s="77"/>
-      <c r="F82" s="77"/>
-      <c r="G82" s="77"/>
-      <c r="H82" s="77"/>
-      <c r="I82" s="77"/>
-      <c r="J82" s="77"/>
-      <c r="K82" s="77"/>
-      <c r="L82" s="77"/>
-      <c r="M82" s="77"/>
-      <c r="N82" s="78"/>
+      <c r="B82" s="75"/>
+      <c r="C82" s="76"/>
+      <c r="D82" s="76"/>
+      <c r="E82" s="76"/>
+      <c r="F82" s="76"/>
+      <c r="G82" s="76"/>
+      <c r="H82" s="76"/>
+      <c r="I82" s="76"/>
+      <c r="J82" s="76"/>
+      <c r="K82" s="76"/>
+      <c r="L82" s="76"/>
+      <c r="M82" s="76"/>
+      <c r="N82" s="77"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B83" s="76"/>
-      <c r="C83" s="77"/>
-      <c r="D83" s="77"/>
-      <c r="E83" s="77"/>
-      <c r="F83" s="77"/>
-      <c r="G83" s="77"/>
-      <c r="H83" s="77"/>
-      <c r="I83" s="77"/>
-      <c r="J83" s="77"/>
-      <c r="K83" s="77"/>
-      <c r="L83" s="77"/>
-      <c r="M83" s="77"/>
-      <c r="N83" s="78"/>
+      <c r="B83" s="75"/>
+      <c r="C83" s="76"/>
+      <c r="D83" s="76"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="76"/>
+      <c r="G83" s="76"/>
+      <c r="H83" s="76"/>
+      <c r="I83" s="76"/>
+      <c r="J83" s="76"/>
+      <c r="K83" s="76"/>
+      <c r="L83" s="76"/>
+      <c r="M83" s="76"/>
+      <c r="N83" s="77"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B84" s="76"/>
-      <c r="C84" s="77"/>
-      <c r="D84" s="77"/>
-      <c r="E84" s="77"/>
-      <c r="F84" s="77"/>
-      <c r="G84" s="77"/>
-      <c r="H84" s="77"/>
-      <c r="I84" s="77"/>
-      <c r="J84" s="77"/>
-      <c r="K84" s="77"/>
-      <c r="L84" s="77"/>
-      <c r="M84" s="77"/>
-      <c r="N84" s="78"/>
+      <c r="B84" s="75"/>
+      <c r="C84" s="76"/>
+      <c r="D84" s="76"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="76"/>
+      <c r="I84" s="76"/>
+      <c r="J84" s="76"/>
+      <c r="K84" s="76"/>
+      <c r="L84" s="76"/>
+      <c r="M84" s="76"/>
+      <c r="N84" s="77"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B85" s="76"/>
-      <c r="C85" s="77"/>
-      <c r="D85" s="77"/>
-      <c r="E85" s="77"/>
-      <c r="F85" s="77"/>
-      <c r="G85" s="77"/>
-      <c r="H85" s="77"/>
-      <c r="I85" s="77"/>
-      <c r="J85" s="77"/>
-      <c r="K85" s="77"/>
-      <c r="L85" s="77"/>
-      <c r="M85" s="77"/>
-      <c r="N85" s="78"/>
+      <c r="B85" s="75"/>
+      <c r="C85" s="76"/>
+      <c r="D85" s="76"/>
+      <c r="E85" s="76"/>
+      <c r="F85" s="76"/>
+      <c r="G85" s="76"/>
+      <c r="H85" s="76"/>
+      <c r="I85" s="76"/>
+      <c r="J85" s="76"/>
+      <c r="K85" s="76"/>
+      <c r="L85" s="76"/>
+      <c r="M85" s="76"/>
+      <c r="N85" s="77"/>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B86" s="76"/>
-      <c r="C86" s="77"/>
-      <c r="D86" s="77"/>
-      <c r="E86" s="77"/>
-      <c r="F86" s="77"/>
-      <c r="G86" s="77"/>
-      <c r="H86" s="77"/>
-      <c r="I86" s="77"/>
-      <c r="J86" s="77"/>
-      <c r="K86" s="77"/>
-      <c r="L86" s="77"/>
-      <c r="M86" s="77"/>
-      <c r="N86" s="78"/>
+      <c r="B86" s="75"/>
+      <c r="C86" s="76"/>
+      <c r="D86" s="76"/>
+      <c r="E86" s="76"/>
+      <c r="F86" s="76"/>
+      <c r="G86" s="76"/>
+      <c r="H86" s="76"/>
+      <c r="I86" s="76"/>
+      <c r="J86" s="76"/>
+      <c r="K86" s="76"/>
+      <c r="L86" s="76"/>
+      <c r="M86" s="76"/>
+      <c r="N86" s="77"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="76"/>
-      <c r="C87" s="77"/>
-      <c r="D87" s="77"/>
-      <c r="E87" s="77"/>
-      <c r="F87" s="77"/>
-      <c r="G87" s="77"/>
-      <c r="H87" s="77"/>
-      <c r="I87" s="77"/>
-      <c r="J87" s="77"/>
-      <c r="K87" s="77"/>
-      <c r="L87" s="77"/>
-      <c r="M87" s="77"/>
-      <c r="N87" s="78"/>
+      <c r="B87" s="75"/>
+      <c r="C87" s="76"/>
+      <c r="D87" s="76"/>
+      <c r="E87" s="76"/>
+      <c r="F87" s="76"/>
+      <c r="G87" s="76"/>
+      <c r="H87" s="76"/>
+      <c r="I87" s="76"/>
+      <c r="J87" s="76"/>
+      <c r="K87" s="76"/>
+      <c r="L87" s="76"/>
+      <c r="M87" s="76"/>
+      <c r="N87" s="77"/>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B88" s="76"/>
-      <c r="C88" s="77"/>
-      <c r="D88" s="77"/>
-      <c r="E88" s="77"/>
-      <c r="F88" s="77"/>
-      <c r="G88" s="77"/>
-      <c r="H88" s="77"/>
-      <c r="I88" s="77"/>
-      <c r="J88" s="77"/>
-      <c r="K88" s="77"/>
-      <c r="L88" s="77"/>
-      <c r="M88" s="77"/>
-      <c r="N88" s="78"/>
+      <c r="B88" s="75"/>
+      <c r="C88" s="76"/>
+      <c r="D88" s="76"/>
+      <c r="E88" s="76"/>
+      <c r="F88" s="76"/>
+      <c r="G88" s="76"/>
+      <c r="H88" s="76"/>
+      <c r="I88" s="76"/>
+      <c r="J88" s="76"/>
+      <c r="K88" s="76"/>
+      <c r="L88" s="76"/>
+      <c r="M88" s="76"/>
+      <c r="N88" s="77"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B89" s="76"/>
-      <c r="C89" s="77"/>
-      <c r="D89" s="77"/>
-      <c r="E89" s="77"/>
-      <c r="F89" s="77"/>
-      <c r="G89" s="77"/>
-      <c r="H89" s="77"/>
-      <c r="I89" s="77"/>
-      <c r="J89" s="77"/>
-      <c r="K89" s="77"/>
-      <c r="L89" s="77"/>
-      <c r="M89" s="77"/>
-      <c r="N89" s="78"/>
+      <c r="B89" s="75"/>
+      <c r="C89" s="76"/>
+      <c r="D89" s="76"/>
+      <c r="E89" s="76"/>
+      <c r="F89" s="76"/>
+      <c r="G89" s="76"/>
+      <c r="H89" s="76"/>
+      <c r="I89" s="76"/>
+      <c r="J89" s="76"/>
+      <c r="K89" s="76"/>
+      <c r="L89" s="76"/>
+      <c r="M89" s="76"/>
+      <c r="N89" s="77"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B90" s="76"/>
-      <c r="C90" s="77"/>
-      <c r="D90" s="77"/>
-      <c r="E90" s="77"/>
-      <c r="F90" s="77"/>
-      <c r="G90" s="77"/>
-      <c r="H90" s="77"/>
-      <c r="I90" s="77"/>
-      <c r="J90" s="77"/>
-      <c r="K90" s="77"/>
-      <c r="L90" s="77"/>
-      <c r="M90" s="77"/>
-      <c r="N90" s="78"/>
+      <c r="B90" s="75"/>
+      <c r="C90" s="76"/>
+      <c r="D90" s="76"/>
+      <c r="E90" s="76"/>
+      <c r="F90" s="76"/>
+      <c r="G90" s="76"/>
+      <c r="H90" s="76"/>
+      <c r="I90" s="76"/>
+      <c r="J90" s="76"/>
+      <c r="K90" s="76"/>
+      <c r="L90" s="76"/>
+      <c r="M90" s="76"/>
+      <c r="N90" s="77"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B91" s="76"/>
-      <c r="C91" s="77"/>
-      <c r="D91" s="77"/>
-      <c r="E91" s="77"/>
-      <c r="F91" s="77"/>
-      <c r="G91" s="77"/>
-      <c r="H91" s="77"/>
-      <c r="I91" s="77"/>
-      <c r="J91" s="77"/>
-      <c r="K91" s="77"/>
-      <c r="L91" s="77"/>
-      <c r="M91" s="77"/>
-      <c r="N91" s="78"/>
+      <c r="B91" s="75"/>
+      <c r="C91" s="76"/>
+      <c r="D91" s="76"/>
+      <c r="E91" s="76"/>
+      <c r="F91" s="76"/>
+      <c r="G91" s="76"/>
+      <c r="H91" s="76"/>
+      <c r="I91" s="76"/>
+      <c r="J91" s="76"/>
+      <c r="K91" s="76"/>
+      <c r="L91" s="76"/>
+      <c r="M91" s="76"/>
+      <c r="N91" s="77"/>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B92" s="76"/>
-      <c r="C92" s="77"/>
-      <c r="D92" s="77"/>
-      <c r="E92" s="77"/>
-      <c r="F92" s="77"/>
-      <c r="G92" s="77"/>
-      <c r="H92" s="77"/>
-      <c r="I92" s="77"/>
-      <c r="J92" s="77"/>
-      <c r="K92" s="77"/>
-      <c r="L92" s="77"/>
-      <c r="M92" s="77"/>
-      <c r="N92" s="78"/>
+      <c r="B92" s="75"/>
+      <c r="C92" s="76"/>
+      <c r="D92" s="76"/>
+      <c r="E92" s="76"/>
+      <c r="F92" s="76"/>
+      <c r="G92" s="76"/>
+      <c r="H92" s="76"/>
+      <c r="I92" s="76"/>
+      <c r="J92" s="76"/>
+      <c r="K92" s="76"/>
+      <c r="L92" s="76"/>
+      <c r="M92" s="76"/>
+      <c r="N92" s="77"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B93" s="76"/>
-      <c r="C93" s="77"/>
-      <c r="D93" s="77"/>
-      <c r="E93" s="77"/>
-      <c r="F93" s="77"/>
-      <c r="G93" s="77"/>
-      <c r="H93" s="77"/>
-      <c r="I93" s="77"/>
-      <c r="J93" s="77"/>
-      <c r="K93" s="77"/>
-      <c r="L93" s="77"/>
-      <c r="M93" s="77"/>
-      <c r="N93" s="78"/>
+      <c r="B93" s="75"/>
+      <c r="C93" s="76"/>
+      <c r="D93" s="76"/>
+      <c r="E93" s="76"/>
+      <c r="F93" s="76"/>
+      <c r="G93" s="76"/>
+      <c r="H93" s="76"/>
+      <c r="I93" s="76"/>
+      <c r="J93" s="76"/>
+      <c r="K93" s="76"/>
+      <c r="L93" s="76"/>
+      <c r="M93" s="76"/>
+      <c r="N93" s="77"/>
     </row>
     <row r="94" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B94" s="76"/>
-      <c r="C94" s="77"/>
-      <c r="D94" s="77"/>
-      <c r="E94" s="77"/>
-      <c r="F94" s="77"/>
-      <c r="G94" s="77"/>
-      <c r="H94" s="77"/>
-      <c r="I94" s="77"/>
-      <c r="J94" s="77"/>
-      <c r="K94" s="77"/>
-      <c r="L94" s="77"/>
-      <c r="M94" s="77"/>
-      <c r="N94" s="78"/>
+      <c r="B94" s="75"/>
+      <c r="C94" s="76"/>
+      <c r="D94" s="76"/>
+      <c r="E94" s="76"/>
+      <c r="F94" s="76"/>
+      <c r="G94" s="76"/>
+      <c r="H94" s="76"/>
+      <c r="I94" s="76"/>
+      <c r="J94" s="76"/>
+      <c r="K94" s="76"/>
+      <c r="L94" s="76"/>
+      <c r="M94" s="76"/>
+      <c r="N94" s="77"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B95" s="76"/>
-      <c r="C95" s="77"/>
-      <c r="D95" s="77"/>
-      <c r="E95" s="77"/>
-      <c r="F95" s="77"/>
-      <c r="G95" s="77"/>
-      <c r="H95" s="77"/>
-      <c r="I95" s="77"/>
-      <c r="J95" s="77"/>
-      <c r="K95" s="77"/>
-      <c r="L95" s="77"/>
-      <c r="M95" s="77"/>
-      <c r="N95" s="78"/>
+      <c r="B95" s="75"/>
+      <c r="C95" s="76"/>
+      <c r="D95" s="76"/>
+      <c r="E95" s="76"/>
+      <c r="F95" s="76"/>
+      <c r="G95" s="76"/>
+      <c r="H95" s="76"/>
+      <c r="I95" s="76"/>
+      <c r="J95" s="76"/>
+      <c r="K95" s="76"/>
+      <c r="L95" s="76"/>
+      <c r="M95" s="76"/>
+      <c r="N95" s="77"/>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B96" s="76"/>
-      <c r="C96" s="77"/>
-      <c r="D96" s="77"/>
-      <c r="E96" s="77"/>
-      <c r="F96" s="77"/>
-      <c r="G96" s="77"/>
-      <c r="H96" s="77"/>
-      <c r="I96" s="77"/>
-      <c r="J96" s="77"/>
-      <c r="K96" s="77"/>
-      <c r="L96" s="77"/>
-      <c r="M96" s="77"/>
-      <c r="N96" s="78"/>
+      <c r="B96" s="75"/>
+      <c r="C96" s="76"/>
+      <c r="D96" s="76"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="76"/>
+      <c r="G96" s="76"/>
+      <c r="H96" s="76"/>
+      <c r="I96" s="76"/>
+      <c r="J96" s="76"/>
+      <c r="K96" s="76"/>
+      <c r="L96" s="76"/>
+      <c r="M96" s="76"/>
+      <c r="N96" s="77"/>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B97" s="76"/>
-      <c r="C97" s="77"/>
-      <c r="D97" s="77"/>
-      <c r="E97" s="77"/>
-      <c r="F97" s="77"/>
-      <c r="G97" s="77"/>
-      <c r="H97" s="77"/>
-      <c r="I97" s="77"/>
-      <c r="J97" s="77"/>
-      <c r="K97" s="77"/>
-      <c r="L97" s="77"/>
-      <c r="M97" s="77"/>
-      <c r="N97" s="78"/>
+      <c r="B97" s="75"/>
+      <c r="C97" s="76"/>
+      <c r="D97" s="76"/>
+      <c r="E97" s="76"/>
+      <c r="F97" s="76"/>
+      <c r="G97" s="76"/>
+      <c r="H97" s="76"/>
+      <c r="I97" s="76"/>
+      <c r="J97" s="76"/>
+      <c r="K97" s="76"/>
+      <c r="L97" s="76"/>
+      <c r="M97" s="76"/>
+      <c r="N97" s="77"/>
     </row>
     <row r="98" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B98" s="76"/>
-      <c r="C98" s="77"/>
-      <c r="D98" s="77"/>
-      <c r="E98" s="77"/>
-      <c r="F98" s="77"/>
-      <c r="G98" s="77"/>
-      <c r="H98" s="77"/>
-      <c r="I98" s="77"/>
-      <c r="J98" s="77"/>
-      <c r="K98" s="77"/>
-      <c r="L98" s="77"/>
-      <c r="M98" s="77"/>
-      <c r="N98" s="78"/>
+      <c r="B98" s="75"/>
+      <c r="C98" s="76"/>
+      <c r="D98" s="76"/>
+      <c r="E98" s="76"/>
+      <c r="F98" s="76"/>
+      <c r="G98" s="76"/>
+      <c r="H98" s="76"/>
+      <c r="I98" s="76"/>
+      <c r="J98" s="76"/>
+      <c r="K98" s="76"/>
+      <c r="L98" s="76"/>
+      <c r="M98" s="76"/>
+      <c r="N98" s="77"/>
     </row>
     <row r="99" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B99" s="76"/>
-      <c r="C99" s="77"/>
-      <c r="D99" s="77"/>
-      <c r="E99" s="77"/>
-      <c r="F99" s="77"/>
-      <c r="G99" s="77"/>
-      <c r="H99" s="77"/>
-      <c r="I99" s="77"/>
-      <c r="J99" s="77"/>
-      <c r="K99" s="77"/>
-      <c r="L99" s="77"/>
-      <c r="M99" s="77"/>
-      <c r="N99" s="78"/>
+      <c r="B99" s="75"/>
+      <c r="C99" s="76"/>
+      <c r="D99" s="76"/>
+      <c r="E99" s="76"/>
+      <c r="F99" s="76"/>
+      <c r="G99" s="76"/>
+      <c r="H99" s="76"/>
+      <c r="I99" s="76"/>
+      <c r="J99" s="76"/>
+      <c r="K99" s="76"/>
+      <c r="L99" s="76"/>
+      <c r="M99" s="76"/>
+      <c r="N99" s="77"/>
     </row>
     <row r="100" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B100" s="76"/>
-      <c r="C100" s="77"/>
-      <c r="D100" s="77"/>
-      <c r="E100" s="77"/>
-      <c r="F100" s="77"/>
-      <c r="G100" s="77"/>
-      <c r="H100" s="77"/>
-      <c r="I100" s="77"/>
-      <c r="J100" s="77"/>
-      <c r="K100" s="77"/>
-      <c r="L100" s="77"/>
-      <c r="M100" s="77"/>
-      <c r="N100" s="78"/>
+      <c r="B100" s="75"/>
+      <c r="C100" s="76"/>
+      <c r="D100" s="76"/>
+      <c r="E100" s="76"/>
+      <c r="F100" s="76"/>
+      <c r="G100" s="76"/>
+      <c r="H100" s="76"/>
+      <c r="I100" s="76"/>
+      <c r="J100" s="76"/>
+      <c r="K100" s="76"/>
+      <c r="L100" s="76"/>
+      <c r="M100" s="76"/>
+      <c r="N100" s="77"/>
     </row>
     <row r="101" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B101" s="76"/>
-      <c r="C101" s="77"/>
-      <c r="D101" s="77"/>
-      <c r="E101" s="77"/>
-      <c r="F101" s="77"/>
-      <c r="G101" s="77"/>
-      <c r="H101" s="77"/>
-      <c r="I101" s="77"/>
-      <c r="J101" s="77"/>
-      <c r="K101" s="77"/>
-      <c r="L101" s="77"/>
-      <c r="M101" s="77"/>
-      <c r="N101" s="78"/>
+      <c r="B101" s="75"/>
+      <c r="C101" s="76"/>
+      <c r="D101" s="76"/>
+      <c r="E101" s="76"/>
+      <c r="F101" s="76"/>
+      <c r="G101" s="76"/>
+      <c r="H101" s="76"/>
+      <c r="I101" s="76"/>
+      <c r="J101" s="76"/>
+      <c r="K101" s="76"/>
+      <c r="L101" s="76"/>
+      <c r="M101" s="76"/>
+      <c r="N101" s="77"/>
     </row>
     <row r="102" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B102" s="76"/>
-      <c r="C102" s="77"/>
-      <c r="D102" s="77"/>
-      <c r="E102" s="77"/>
-      <c r="F102" s="77"/>
-      <c r="G102" s="77"/>
-      <c r="H102" s="77"/>
-      <c r="I102" s="77"/>
-      <c r="J102" s="77"/>
-      <c r="K102" s="77"/>
-      <c r="L102" s="77"/>
-      <c r="M102" s="77"/>
-      <c r="N102" s="78"/>
+      <c r="B102" s="75"/>
+      <c r="C102" s="76"/>
+      <c r="D102" s="76"/>
+      <c r="E102" s="76"/>
+      <c r="F102" s="76"/>
+      <c r="G102" s="76"/>
+      <c r="H102" s="76"/>
+      <c r="I102" s="76"/>
+      <c r="J102" s="76"/>
+      <c r="K102" s="76"/>
+      <c r="L102" s="76"/>
+      <c r="M102" s="76"/>
+      <c r="N102" s="77"/>
     </row>
     <row r="103" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B103" s="76"/>
-      <c r="C103" s="77"/>
-      <c r="D103" s="77"/>
-      <c r="E103" s="77"/>
-      <c r="F103" s="77"/>
-      <c r="G103" s="77"/>
-      <c r="H103" s="77"/>
-      <c r="I103" s="77"/>
-      <c r="J103" s="77"/>
-      <c r="K103" s="77"/>
-      <c r="L103" s="77"/>
-      <c r="M103" s="77"/>
-      <c r="N103" s="78"/>
+      <c r="B103" s="75"/>
+      <c r="C103" s="76"/>
+      <c r="D103" s="76"/>
+      <c r="E103" s="76"/>
+      <c r="F103" s="76"/>
+      <c r="G103" s="76"/>
+      <c r="H103" s="76"/>
+      <c r="I103" s="76"/>
+      <c r="J103" s="76"/>
+      <c r="K103" s="76"/>
+      <c r="L103" s="76"/>
+      <c r="M103" s="76"/>
+      <c r="N103" s="77"/>
     </row>
     <row r="104" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B104" s="79"/>
-      <c r="C104" s="80"/>
-      <c r="D104" s="80"/>
-      <c r="E104" s="80"/>
-      <c r="F104" s="80"/>
-      <c r="G104" s="80"/>
-      <c r="H104" s="80"/>
-      <c r="I104" s="80"/>
-      <c r="J104" s="80"/>
-      <c r="K104" s="80"/>
-      <c r="L104" s="80"/>
-      <c r="M104" s="80"/>
-      <c r="N104" s="81"/>
+      <c r="B104" s="78"/>
+      <c r="C104" s="79"/>
+      <c r="D104" s="79"/>
+      <c r="E104" s="79"/>
+      <c r="F104" s="79"/>
+      <c r="G104" s="79"/>
+      <c r="H104" s="79"/>
+      <c r="I104" s="79"/>
+      <c r="J104" s="79"/>
+      <c r="K104" s="79"/>
+      <c r="L104" s="79"/>
+      <c r="M104" s="79"/>
+      <c r="N104" s="80"/>
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B105" s="71" t="s">
@@ -4315,452 +4315,452 @@
       <c r="N105" s="71"/>
     </row>
     <row r="106" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B106" s="73"/>
-      <c r="C106" s="74"/>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="74"/>
-      <c r="H106" s="74"/>
-      <c r="I106" s="74"/>
-      <c r="J106" s="74"/>
-      <c r="K106" s="74"/>
-      <c r="L106" s="74"/>
-      <c r="M106" s="74"/>
-      <c r="N106" s="75"/>
+      <c r="B106" s="72"/>
+      <c r="C106" s="73"/>
+      <c r="D106" s="73"/>
+      <c r="E106" s="73"/>
+      <c r="F106" s="73"/>
+      <c r="G106" s="73"/>
+      <c r="H106" s="73"/>
+      <c r="I106" s="73"/>
+      <c r="J106" s="73"/>
+      <c r="K106" s="73"/>
+      <c r="L106" s="73"/>
+      <c r="M106" s="73"/>
+      <c r="N106" s="74"/>
     </row>
     <row r="107" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B107" s="76"/>
-      <c r="C107" s="77"/>
-      <c r="D107" s="77"/>
-      <c r="E107" s="77"/>
-      <c r="F107" s="77"/>
-      <c r="G107" s="77"/>
-      <c r="H107" s="77"/>
-      <c r="I107" s="77"/>
-      <c r="J107" s="77"/>
-      <c r="K107" s="77"/>
-      <c r="L107" s="77"/>
-      <c r="M107" s="77"/>
-      <c r="N107" s="78"/>
+      <c r="B107" s="75"/>
+      <c r="C107" s="76"/>
+      <c r="D107" s="76"/>
+      <c r="E107" s="76"/>
+      <c r="F107" s="76"/>
+      <c r="G107" s="76"/>
+      <c r="H107" s="76"/>
+      <c r="I107" s="76"/>
+      <c r="J107" s="76"/>
+      <c r="K107" s="76"/>
+      <c r="L107" s="76"/>
+      <c r="M107" s="76"/>
+      <c r="N107" s="77"/>
     </row>
     <row r="108" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B108" s="76"/>
-      <c r="C108" s="77"/>
-      <c r="D108" s="77"/>
-      <c r="E108" s="77"/>
-      <c r="F108" s="77"/>
-      <c r="G108" s="77"/>
-      <c r="H108" s="77"/>
-      <c r="I108" s="77"/>
-      <c r="J108" s="77"/>
-      <c r="K108" s="77"/>
-      <c r="L108" s="77"/>
-      <c r="M108" s="77"/>
-      <c r="N108" s="78"/>
+      <c r="B108" s="75"/>
+      <c r="C108" s="76"/>
+      <c r="D108" s="76"/>
+      <c r="E108" s="76"/>
+      <c r="F108" s="76"/>
+      <c r="G108" s="76"/>
+      <c r="H108" s="76"/>
+      <c r="I108" s="76"/>
+      <c r="J108" s="76"/>
+      <c r="K108" s="76"/>
+      <c r="L108" s="76"/>
+      <c r="M108" s="76"/>
+      <c r="N108" s="77"/>
     </row>
     <row r="109" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B109" s="76"/>
-      <c r="C109" s="77"/>
-      <c r="D109" s="77"/>
-      <c r="E109" s="77"/>
-      <c r="F109" s="77"/>
-      <c r="G109" s="77"/>
-      <c r="H109" s="77"/>
-      <c r="I109" s="77"/>
-      <c r="J109" s="77"/>
-      <c r="K109" s="77"/>
-      <c r="L109" s="77"/>
-      <c r="M109" s="77"/>
-      <c r="N109" s="78"/>
+      <c r="B109" s="75"/>
+      <c r="C109" s="76"/>
+      <c r="D109" s="76"/>
+      <c r="E109" s="76"/>
+      <c r="F109" s="76"/>
+      <c r="G109" s="76"/>
+      <c r="H109" s="76"/>
+      <c r="I109" s="76"/>
+      <c r="J109" s="76"/>
+      <c r="K109" s="76"/>
+      <c r="L109" s="76"/>
+      <c r="M109" s="76"/>
+      <c r="N109" s="77"/>
     </row>
     <row r="110" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B110" s="76"/>
-      <c r="C110" s="77"/>
-      <c r="D110" s="77"/>
-      <c r="E110" s="77"/>
-      <c r="F110" s="77"/>
-      <c r="G110" s="77"/>
-      <c r="H110" s="77"/>
-      <c r="I110" s="77"/>
-      <c r="J110" s="77"/>
-      <c r="K110" s="77"/>
-      <c r="L110" s="77"/>
-      <c r="M110" s="77"/>
-      <c r="N110" s="78"/>
+      <c r="B110" s="75"/>
+      <c r="C110" s="76"/>
+      <c r="D110" s="76"/>
+      <c r="E110" s="76"/>
+      <c r="F110" s="76"/>
+      <c r="G110" s="76"/>
+      <c r="H110" s="76"/>
+      <c r="I110" s="76"/>
+      <c r="J110" s="76"/>
+      <c r="K110" s="76"/>
+      <c r="L110" s="76"/>
+      <c r="M110" s="76"/>
+      <c r="N110" s="77"/>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B111" s="76"/>
-      <c r="C111" s="77"/>
-      <c r="D111" s="77"/>
-      <c r="E111" s="77"/>
-      <c r="F111" s="77"/>
-      <c r="G111" s="77"/>
-      <c r="H111" s="77"/>
-      <c r="I111" s="77"/>
-      <c r="J111" s="77"/>
-      <c r="K111" s="77"/>
-      <c r="L111" s="77"/>
-      <c r="M111" s="77"/>
-      <c r="N111" s="78"/>
+      <c r="B111" s="75"/>
+      <c r="C111" s="76"/>
+      <c r="D111" s="76"/>
+      <c r="E111" s="76"/>
+      <c r="F111" s="76"/>
+      <c r="G111" s="76"/>
+      <c r="H111" s="76"/>
+      <c r="I111" s="76"/>
+      <c r="J111" s="76"/>
+      <c r="K111" s="76"/>
+      <c r="L111" s="76"/>
+      <c r="M111" s="76"/>
+      <c r="N111" s="77"/>
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B112" s="76"/>
-      <c r="C112" s="77"/>
-      <c r="D112" s="77"/>
-      <c r="E112" s="77"/>
-      <c r="F112" s="77"/>
-      <c r="G112" s="77"/>
-      <c r="H112" s="77"/>
-      <c r="I112" s="77"/>
-      <c r="J112" s="77"/>
-      <c r="K112" s="77"/>
-      <c r="L112" s="77"/>
-      <c r="M112" s="77"/>
-      <c r="N112" s="78"/>
+      <c r="B112" s="75"/>
+      <c r="C112" s="76"/>
+      <c r="D112" s="76"/>
+      <c r="E112" s="76"/>
+      <c r="F112" s="76"/>
+      <c r="G112" s="76"/>
+      <c r="H112" s="76"/>
+      <c r="I112" s="76"/>
+      <c r="J112" s="76"/>
+      <c r="K112" s="76"/>
+      <c r="L112" s="76"/>
+      <c r="M112" s="76"/>
+      <c r="N112" s="77"/>
     </row>
     <row r="113" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B113" s="76"/>
-      <c r="C113" s="77"/>
-      <c r="D113" s="77"/>
-      <c r="E113" s="77"/>
-      <c r="F113" s="77"/>
-      <c r="G113" s="77"/>
-      <c r="H113" s="77"/>
-      <c r="I113" s="77"/>
-      <c r="J113" s="77"/>
-      <c r="K113" s="77"/>
-      <c r="L113" s="77"/>
-      <c r="M113" s="77"/>
-      <c r="N113" s="78"/>
+      <c r="B113" s="75"/>
+      <c r="C113" s="76"/>
+      <c r="D113" s="76"/>
+      <c r="E113" s="76"/>
+      <c r="F113" s="76"/>
+      <c r="G113" s="76"/>
+      <c r="H113" s="76"/>
+      <c r="I113" s="76"/>
+      <c r="J113" s="76"/>
+      <c r="K113" s="76"/>
+      <c r="L113" s="76"/>
+      <c r="M113" s="76"/>
+      <c r="N113" s="77"/>
     </row>
     <row r="114" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B114" s="76"/>
-      <c r="C114" s="77"/>
-      <c r="D114" s="77"/>
-      <c r="E114" s="77"/>
-      <c r="F114" s="77"/>
-      <c r="G114" s="77"/>
-      <c r="H114" s="77"/>
-      <c r="I114" s="77"/>
-      <c r="J114" s="77"/>
-      <c r="K114" s="77"/>
-      <c r="L114" s="77"/>
-      <c r="M114" s="77"/>
-      <c r="N114" s="78"/>
+      <c r="B114" s="75"/>
+      <c r="C114" s="76"/>
+      <c r="D114" s="76"/>
+      <c r="E114" s="76"/>
+      <c r="F114" s="76"/>
+      <c r="G114" s="76"/>
+      <c r="H114" s="76"/>
+      <c r="I114" s="76"/>
+      <c r="J114" s="76"/>
+      <c r="K114" s="76"/>
+      <c r="L114" s="76"/>
+      <c r="M114" s="76"/>
+      <c r="N114" s="77"/>
     </row>
     <row r="115" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B115" s="76"/>
-      <c r="C115" s="77"/>
-      <c r="D115" s="77"/>
-      <c r="E115" s="77"/>
-      <c r="F115" s="77"/>
-      <c r="G115" s="77"/>
-      <c r="H115" s="77"/>
-      <c r="I115" s="77"/>
-      <c r="J115" s="77"/>
-      <c r="K115" s="77"/>
-      <c r="L115" s="77"/>
-      <c r="M115" s="77"/>
-      <c r="N115" s="78"/>
+      <c r="B115" s="75"/>
+      <c r="C115" s="76"/>
+      <c r="D115" s="76"/>
+      <c r="E115" s="76"/>
+      <c r="F115" s="76"/>
+      <c r="G115" s="76"/>
+      <c r="H115" s="76"/>
+      <c r="I115" s="76"/>
+      <c r="J115" s="76"/>
+      <c r="K115" s="76"/>
+      <c r="L115" s="76"/>
+      <c r="M115" s="76"/>
+      <c r="N115" s="77"/>
     </row>
     <row r="116" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B116" s="76"/>
-      <c r="C116" s="77"/>
-      <c r="D116" s="77"/>
-      <c r="E116" s="77"/>
-      <c r="F116" s="77"/>
-      <c r="G116" s="77"/>
-      <c r="H116" s="77"/>
-      <c r="I116" s="77"/>
-      <c r="J116" s="77"/>
-      <c r="K116" s="77"/>
-      <c r="L116" s="77"/>
-      <c r="M116" s="77"/>
-      <c r="N116" s="78"/>
+      <c r="B116" s="75"/>
+      <c r="C116" s="76"/>
+      <c r="D116" s="76"/>
+      <c r="E116" s="76"/>
+      <c r="F116" s="76"/>
+      <c r="G116" s="76"/>
+      <c r="H116" s="76"/>
+      <c r="I116" s="76"/>
+      <c r="J116" s="76"/>
+      <c r="K116" s="76"/>
+      <c r="L116" s="76"/>
+      <c r="M116" s="76"/>
+      <c r="N116" s="77"/>
     </row>
     <row r="117" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B117" s="76"/>
-      <c r="C117" s="77"/>
-      <c r="D117" s="77"/>
-      <c r="E117" s="77"/>
-      <c r="F117" s="77"/>
-      <c r="G117" s="77"/>
-      <c r="H117" s="77"/>
-      <c r="I117" s="77"/>
-      <c r="J117" s="77"/>
-      <c r="K117" s="77"/>
-      <c r="L117" s="77"/>
-      <c r="M117" s="77"/>
-      <c r="N117" s="78"/>
+      <c r="B117" s="75"/>
+      <c r="C117" s="76"/>
+      <c r="D117" s="76"/>
+      <c r="E117" s="76"/>
+      <c r="F117" s="76"/>
+      <c r="G117" s="76"/>
+      <c r="H117" s="76"/>
+      <c r="I117" s="76"/>
+      <c r="J117" s="76"/>
+      <c r="K117" s="76"/>
+      <c r="L117" s="76"/>
+      <c r="M117" s="76"/>
+      <c r="N117" s="77"/>
     </row>
     <row r="118" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B118" s="76"/>
-      <c r="C118" s="77"/>
-      <c r="D118" s="77"/>
-      <c r="E118" s="77"/>
-      <c r="F118" s="77"/>
-      <c r="G118" s="77"/>
-      <c r="H118" s="77"/>
-      <c r="I118" s="77"/>
-      <c r="J118" s="77"/>
-      <c r="K118" s="77"/>
-      <c r="L118" s="77"/>
-      <c r="M118" s="77"/>
-      <c r="N118" s="78"/>
+      <c r="B118" s="75"/>
+      <c r="C118" s="76"/>
+      <c r="D118" s="76"/>
+      <c r="E118" s="76"/>
+      <c r="F118" s="76"/>
+      <c r="G118" s="76"/>
+      <c r="H118" s="76"/>
+      <c r="I118" s="76"/>
+      <c r="J118" s="76"/>
+      <c r="K118" s="76"/>
+      <c r="L118" s="76"/>
+      <c r="M118" s="76"/>
+      <c r="N118" s="77"/>
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B119" s="76"/>
-      <c r="C119" s="77"/>
-      <c r="D119" s="77"/>
-      <c r="E119" s="77"/>
-      <c r="F119" s="77"/>
-      <c r="G119" s="77"/>
-      <c r="H119" s="77"/>
-      <c r="I119" s="77"/>
-      <c r="J119" s="77"/>
-      <c r="K119" s="77"/>
-      <c r="L119" s="77"/>
-      <c r="M119" s="77"/>
-      <c r="N119" s="78"/>
+      <c r="B119" s="75"/>
+      <c r="C119" s="76"/>
+      <c r="D119" s="76"/>
+      <c r="E119" s="76"/>
+      <c r="F119" s="76"/>
+      <c r="G119" s="76"/>
+      <c r="H119" s="76"/>
+      <c r="I119" s="76"/>
+      <c r="J119" s="76"/>
+      <c r="K119" s="76"/>
+      <c r="L119" s="76"/>
+      <c r="M119" s="76"/>
+      <c r="N119" s="77"/>
     </row>
     <row r="120" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B120" s="76"/>
-      <c r="C120" s="77"/>
-      <c r="D120" s="77"/>
-      <c r="E120" s="77"/>
-      <c r="F120" s="77"/>
-      <c r="G120" s="77"/>
-      <c r="H120" s="77"/>
-      <c r="I120" s="77"/>
-      <c r="J120" s="77"/>
-      <c r="K120" s="77"/>
-      <c r="L120" s="77"/>
-      <c r="M120" s="77"/>
-      <c r="N120" s="78"/>
+      <c r="B120" s="75"/>
+      <c r="C120" s="76"/>
+      <c r="D120" s="76"/>
+      <c r="E120" s="76"/>
+      <c r="F120" s="76"/>
+      <c r="G120" s="76"/>
+      <c r="H120" s="76"/>
+      <c r="I120" s="76"/>
+      <c r="J120" s="76"/>
+      <c r="K120" s="76"/>
+      <c r="L120" s="76"/>
+      <c r="M120" s="76"/>
+      <c r="N120" s="77"/>
     </row>
     <row r="121" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B121" s="76"/>
-      <c r="C121" s="77"/>
-      <c r="D121" s="77"/>
-      <c r="E121" s="77"/>
-      <c r="F121" s="77"/>
-      <c r="G121" s="77"/>
-      <c r="H121" s="77"/>
-      <c r="I121" s="77"/>
-      <c r="J121" s="77"/>
-      <c r="K121" s="77"/>
-      <c r="L121" s="77"/>
-      <c r="M121" s="77"/>
-      <c r="N121" s="78"/>
+      <c r="B121" s="75"/>
+      <c r="C121" s="76"/>
+      <c r="D121" s="76"/>
+      <c r="E121" s="76"/>
+      <c r="F121" s="76"/>
+      <c r="G121" s="76"/>
+      <c r="H121" s="76"/>
+      <c r="I121" s="76"/>
+      <c r="J121" s="76"/>
+      <c r="K121" s="76"/>
+      <c r="L121" s="76"/>
+      <c r="M121" s="76"/>
+      <c r="N121" s="77"/>
     </row>
     <row r="122" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B122" s="76"/>
-      <c r="C122" s="77"/>
-      <c r="D122" s="77"/>
-      <c r="E122" s="77"/>
-      <c r="F122" s="77"/>
-      <c r="G122" s="77"/>
-      <c r="H122" s="77"/>
-      <c r="I122" s="77"/>
-      <c r="J122" s="77"/>
-      <c r="K122" s="77"/>
-      <c r="L122" s="77"/>
-      <c r="M122" s="77"/>
-      <c r="N122" s="78"/>
+      <c r="B122" s="75"/>
+      <c r="C122" s="76"/>
+      <c r="D122" s="76"/>
+      <c r="E122" s="76"/>
+      <c r="F122" s="76"/>
+      <c r="G122" s="76"/>
+      <c r="H122" s="76"/>
+      <c r="I122" s="76"/>
+      <c r="J122" s="76"/>
+      <c r="K122" s="76"/>
+      <c r="L122" s="76"/>
+      <c r="M122" s="76"/>
+      <c r="N122" s="77"/>
     </row>
     <row r="123" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B123" s="76"/>
-      <c r="C123" s="77"/>
-      <c r="D123" s="77"/>
-      <c r="E123" s="77"/>
-      <c r="F123" s="77"/>
-      <c r="G123" s="77"/>
-      <c r="H123" s="77"/>
-      <c r="I123" s="77"/>
-      <c r="J123" s="77"/>
-      <c r="K123" s="77"/>
-      <c r="L123" s="77"/>
-      <c r="M123" s="77"/>
-      <c r="N123" s="78"/>
+      <c r="B123" s="75"/>
+      <c r="C123" s="76"/>
+      <c r="D123" s="76"/>
+      <c r="E123" s="76"/>
+      <c r="F123" s="76"/>
+      <c r="G123" s="76"/>
+      <c r="H123" s="76"/>
+      <c r="I123" s="76"/>
+      <c r="J123" s="76"/>
+      <c r="K123" s="76"/>
+      <c r="L123" s="76"/>
+      <c r="M123" s="76"/>
+      <c r="N123" s="77"/>
     </row>
     <row r="124" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B124" s="76"/>
-      <c r="C124" s="77"/>
-      <c r="D124" s="77"/>
-      <c r="E124" s="77"/>
-      <c r="F124" s="77"/>
-      <c r="G124" s="77"/>
-      <c r="H124" s="77"/>
-      <c r="I124" s="77"/>
-      <c r="J124" s="77"/>
-      <c r="K124" s="77"/>
-      <c r="L124" s="77"/>
-      <c r="M124" s="77"/>
-      <c r="N124" s="78"/>
+      <c r="B124" s="75"/>
+      <c r="C124" s="76"/>
+      <c r="D124" s="76"/>
+      <c r="E124" s="76"/>
+      <c r="F124" s="76"/>
+      <c r="G124" s="76"/>
+      <c r="H124" s="76"/>
+      <c r="I124" s="76"/>
+      <c r="J124" s="76"/>
+      <c r="K124" s="76"/>
+      <c r="L124" s="76"/>
+      <c r="M124" s="76"/>
+      <c r="N124" s="77"/>
     </row>
     <row r="125" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B125" s="76"/>
-      <c r="C125" s="77"/>
-      <c r="D125" s="77"/>
-      <c r="E125" s="77"/>
-      <c r="F125" s="77"/>
-      <c r="G125" s="77"/>
-      <c r="H125" s="77"/>
-      <c r="I125" s="77"/>
-      <c r="J125" s="77"/>
-      <c r="K125" s="77"/>
-      <c r="L125" s="77"/>
-      <c r="M125" s="77"/>
-      <c r="N125" s="78"/>
+      <c r="B125" s="75"/>
+      <c r="C125" s="76"/>
+      <c r="D125" s="76"/>
+      <c r="E125" s="76"/>
+      <c r="F125" s="76"/>
+      <c r="G125" s="76"/>
+      <c r="H125" s="76"/>
+      <c r="I125" s="76"/>
+      <c r="J125" s="76"/>
+      <c r="K125" s="76"/>
+      <c r="L125" s="76"/>
+      <c r="M125" s="76"/>
+      <c r="N125" s="77"/>
     </row>
     <row r="126" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B126" s="76"/>
-      <c r="C126" s="77"/>
-      <c r="D126" s="77"/>
-      <c r="E126" s="77"/>
-      <c r="F126" s="77"/>
-      <c r="G126" s="77"/>
-      <c r="H126" s="77"/>
-      <c r="I126" s="77"/>
-      <c r="J126" s="77"/>
-      <c r="K126" s="77"/>
-      <c r="L126" s="77"/>
-      <c r="M126" s="77"/>
-      <c r="N126" s="78"/>
+      <c r="B126" s="75"/>
+      <c r="C126" s="76"/>
+      <c r="D126" s="76"/>
+      <c r="E126" s="76"/>
+      <c r="F126" s="76"/>
+      <c r="G126" s="76"/>
+      <c r="H126" s="76"/>
+      <c r="I126" s="76"/>
+      <c r="J126" s="76"/>
+      <c r="K126" s="76"/>
+      <c r="L126" s="76"/>
+      <c r="M126" s="76"/>
+      <c r="N126" s="77"/>
     </row>
     <row r="127" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B127" s="76"/>
-      <c r="C127" s="77"/>
-      <c r="D127" s="77"/>
-      <c r="E127" s="77"/>
-      <c r="F127" s="77"/>
-      <c r="G127" s="77"/>
-      <c r="H127" s="77"/>
-      <c r="I127" s="77"/>
-      <c r="J127" s="77"/>
-      <c r="K127" s="77"/>
-      <c r="L127" s="77"/>
-      <c r="M127" s="77"/>
-      <c r="N127" s="78"/>
+      <c r="B127" s="75"/>
+      <c r="C127" s="76"/>
+      <c r="D127" s="76"/>
+      <c r="E127" s="76"/>
+      <c r="F127" s="76"/>
+      <c r="G127" s="76"/>
+      <c r="H127" s="76"/>
+      <c r="I127" s="76"/>
+      <c r="J127" s="76"/>
+      <c r="K127" s="76"/>
+      <c r="L127" s="76"/>
+      <c r="M127" s="76"/>
+      <c r="N127" s="77"/>
     </row>
     <row r="128" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B128" s="76"/>
-      <c r="C128" s="77"/>
-      <c r="D128" s="77"/>
-      <c r="E128" s="77"/>
-      <c r="F128" s="77"/>
-      <c r="G128" s="77"/>
-      <c r="H128" s="77"/>
-      <c r="I128" s="77"/>
-      <c r="J128" s="77"/>
-      <c r="K128" s="77"/>
-      <c r="L128" s="77"/>
-      <c r="M128" s="77"/>
-      <c r="N128" s="78"/>
+      <c r="B128" s="75"/>
+      <c r="C128" s="76"/>
+      <c r="D128" s="76"/>
+      <c r="E128" s="76"/>
+      <c r="F128" s="76"/>
+      <c r="G128" s="76"/>
+      <c r="H128" s="76"/>
+      <c r="I128" s="76"/>
+      <c r="J128" s="76"/>
+      <c r="K128" s="76"/>
+      <c r="L128" s="76"/>
+      <c r="M128" s="76"/>
+      <c r="N128" s="77"/>
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B129" s="76"/>
-      <c r="C129" s="77"/>
-      <c r="D129" s="77"/>
-      <c r="E129" s="77"/>
-      <c r="F129" s="77"/>
-      <c r="G129" s="77"/>
-      <c r="H129" s="77"/>
-      <c r="I129" s="77"/>
-      <c r="J129" s="77"/>
-      <c r="K129" s="77"/>
-      <c r="L129" s="77"/>
-      <c r="M129" s="77"/>
-      <c r="N129" s="78"/>
+      <c r="B129" s="75"/>
+      <c r="C129" s="76"/>
+      <c r="D129" s="76"/>
+      <c r="E129" s="76"/>
+      <c r="F129" s="76"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="76"/>
+      <c r="I129" s="76"/>
+      <c r="J129" s="76"/>
+      <c r="K129" s="76"/>
+      <c r="L129" s="76"/>
+      <c r="M129" s="76"/>
+      <c r="N129" s="77"/>
     </row>
     <row r="130" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B130" s="76"/>
-      <c r="C130" s="77"/>
-      <c r="D130" s="77"/>
-      <c r="E130" s="77"/>
-      <c r="F130" s="77"/>
-      <c r="G130" s="77"/>
-      <c r="H130" s="77"/>
-      <c r="I130" s="77"/>
-      <c r="J130" s="77"/>
-      <c r="K130" s="77"/>
-      <c r="L130" s="77"/>
-      <c r="M130" s="77"/>
-      <c r="N130" s="78"/>
+      <c r="B130" s="75"/>
+      <c r="C130" s="76"/>
+      <c r="D130" s="76"/>
+      <c r="E130" s="76"/>
+      <c r="F130" s="76"/>
+      <c r="G130" s="76"/>
+      <c r="H130" s="76"/>
+      <c r="I130" s="76"/>
+      <c r="J130" s="76"/>
+      <c r="K130" s="76"/>
+      <c r="L130" s="76"/>
+      <c r="M130" s="76"/>
+      <c r="N130" s="77"/>
     </row>
     <row r="131" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B131" s="76"/>
-      <c r="C131" s="77"/>
-      <c r="D131" s="77"/>
-      <c r="E131" s="77"/>
-      <c r="F131" s="77"/>
-      <c r="G131" s="77"/>
-      <c r="H131" s="77"/>
-      <c r="I131" s="77"/>
-      <c r="J131" s="77"/>
-      <c r="K131" s="77"/>
-      <c r="L131" s="77"/>
-      <c r="M131" s="77"/>
-      <c r="N131" s="78"/>
+      <c r="B131" s="75"/>
+      <c r="C131" s="76"/>
+      <c r="D131" s="76"/>
+      <c r="E131" s="76"/>
+      <c r="F131" s="76"/>
+      <c r="G131" s="76"/>
+      <c r="H131" s="76"/>
+      <c r="I131" s="76"/>
+      <c r="J131" s="76"/>
+      <c r="K131" s="76"/>
+      <c r="L131" s="76"/>
+      <c r="M131" s="76"/>
+      <c r="N131" s="77"/>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B132" s="76"/>
-      <c r="C132" s="77"/>
-      <c r="D132" s="77"/>
-      <c r="E132" s="77"/>
-      <c r="F132" s="77"/>
-      <c r="G132" s="77"/>
-      <c r="H132" s="77"/>
-      <c r="I132" s="77"/>
-      <c r="J132" s="77"/>
-      <c r="K132" s="77"/>
-      <c r="L132" s="77"/>
-      <c r="M132" s="77"/>
-      <c r="N132" s="78"/>
+      <c r="B132" s="75"/>
+      <c r="C132" s="76"/>
+      <c r="D132" s="76"/>
+      <c r="E132" s="76"/>
+      <c r="F132" s="76"/>
+      <c r="G132" s="76"/>
+      <c r="H132" s="76"/>
+      <c r="I132" s="76"/>
+      <c r="J132" s="76"/>
+      <c r="K132" s="76"/>
+      <c r="L132" s="76"/>
+      <c r="M132" s="76"/>
+      <c r="N132" s="77"/>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B133" s="76"/>
-      <c r="C133" s="77"/>
-      <c r="D133" s="77"/>
-      <c r="E133" s="77"/>
-      <c r="F133" s="77"/>
-      <c r="G133" s="77"/>
-      <c r="H133" s="77"/>
-      <c r="I133" s="77"/>
-      <c r="J133" s="77"/>
-      <c r="K133" s="77"/>
-      <c r="L133" s="77"/>
-      <c r="M133" s="77"/>
-      <c r="N133" s="78"/>
+      <c r="B133" s="75"/>
+      <c r="C133" s="76"/>
+      <c r="D133" s="76"/>
+      <c r="E133" s="76"/>
+      <c r="F133" s="76"/>
+      <c r="G133" s="76"/>
+      <c r="H133" s="76"/>
+      <c r="I133" s="76"/>
+      <c r="J133" s="76"/>
+      <c r="K133" s="76"/>
+      <c r="L133" s="76"/>
+      <c r="M133" s="76"/>
+      <c r="N133" s="77"/>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B134" s="79"/>
-      <c r="C134" s="80"/>
-      <c r="D134" s="80"/>
-      <c r="E134" s="80"/>
-      <c r="F134" s="80"/>
-      <c r="G134" s="80"/>
-      <c r="H134" s="80"/>
-      <c r="I134" s="80"/>
-      <c r="J134" s="80"/>
-      <c r="K134" s="80"/>
-      <c r="L134" s="80"/>
-      <c r="M134" s="80"/>
-      <c r="N134" s="81"/>
+      <c r="B134" s="78"/>
+      <c r="C134" s="79"/>
+      <c r="D134" s="79"/>
+      <c r="E134" s="79"/>
+      <c r="F134" s="79"/>
+      <c r="G134" s="79"/>
+      <c r="H134" s="79"/>
+      <c r="I134" s="79"/>
+      <c r="J134" s="79"/>
+      <c r="K134" s="79"/>
+      <c r="L134" s="79"/>
+      <c r="M134" s="79"/>
+      <c r="N134" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="B2:N20"/>
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="B22:N44"/>
+    <mergeCell ref="B45:N45"/>
     <mergeCell ref="B75:N75"/>
     <mergeCell ref="B76:N104"/>
     <mergeCell ref="B105:N105"/>
     <mergeCell ref="B106:N134"/>
     <mergeCell ref="B46:N74"/>
-    <mergeCell ref="B21:N21"/>
-    <mergeCell ref="B2:N20"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B22:N44"/>
-    <mergeCell ref="B45:N45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4785,12 +4785,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -4827,10 +4827,10 @@
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="86"/>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -4839,10 +4839,10 @@
       <c r="B5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="83"/>
+      <c r="D5" s="85"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -4879,10 +4879,10 @@
       <c r="B8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="85" t="s">
+      <c r="C8" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="86"/>
+      <c r="D8" s="88"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
@@ -4891,10 +4891,10 @@
       <c r="B9" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="88"/>
+      <c r="D9" s="83"/>
     </row>
     <row r="10" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
@@ -4903,10 +4903,10 @@
       <c r="B10" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="88"/>
+      <c r="D10" s="83"/>
     </row>
     <row r="11" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
@@ -4915,10 +4915,10 @@
       <c r="B11" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="82" t="s">
         <v>194</v>
       </c>
-      <c r="D11" s="88"/>
+      <c r="D11" s="83"/>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
@@ -4927,10 +4927,10 @@
       <c r="B12" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="82" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="88"/>
+      <c r="D12" s="83"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -4967,10 +4967,10 @@
       <c r="B15" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="82"/>
+      <c r="D15" s="84"/>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -4979,10 +4979,10 @@
       <c r="B16" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="83" t="s">
+      <c r="C16" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="83"/>
+      <c r="D16" s="85"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
@@ -5019,10 +5019,10 @@
       <c r="B19" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="82"/>
+      <c r="D19" s="84"/>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
@@ -5031,10 +5031,10 @@
       <c r="B20" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="83" t="s">
+      <c r="C20" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="D20" s="83"/>
+      <c r="D20" s="85"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
@@ -5071,10 +5071,10 @@
       <c r="B23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="82"/>
+      <c r="D23" s="84"/>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
@@ -5083,10 +5083,10 @@
       <c r="B24" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="C24" s="83" t="s">
+      <c r="C24" s="85" t="s">
         <v>200</v>
       </c>
-      <c r="D24" s="83"/>
+      <c r="D24" s="85"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
@@ -5135,10 +5135,10 @@
       <c r="B28" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="82" t="s">
+      <c r="C28" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="82"/>
+      <c r="D28" s="84"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
@@ -5147,10 +5147,10 @@
       <c r="B29" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="85" t="s">
         <v>201</v>
       </c>
-      <c r="D29" s="83"/>
+      <c r="D29" s="85"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
@@ -5187,10 +5187,10 @@
       <c r="B32" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="82" t="s">
+      <c r="C32" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="82"/>
+      <c r="D32" s="84"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
@@ -5199,10 +5199,10 @@
       <c r="B33" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="C33" s="83" t="s">
+      <c r="C33" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="83"/>
+      <c r="D33" s="85"/>
     </row>
     <row r="34" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
@@ -5211,10 +5211,10 @@
       <c r="B34" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="88"/>
+      <c r="D34" s="83"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
@@ -5251,10 +5251,10 @@
       <c r="B37" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="82" t="s">
+      <c r="C37" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="82"/>
+      <c r="D37" s="84"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
@@ -5263,10 +5263,10 @@
       <c r="B38" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="83" t="s">
+      <c r="C38" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="83"/>
+      <c r="D38" s="85"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
@@ -5275,10 +5275,10 @@
       <c r="B39" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C39" s="83" t="s">
+      <c r="C39" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="83"/>
+      <c r="D39" s="85"/>
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
@@ -5287,10 +5287,10 @@
       <c r="B40" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="C40" s="87" t="s">
+      <c r="C40" s="82" t="s">
         <v>226</v>
       </c>
-      <c r="D40" s="88"/>
+      <c r="D40" s="83"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
@@ -5327,10 +5327,10 @@
       <c r="B43" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="82" t="s">
+      <c r="C43" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="82"/>
+      <c r="D43" s="84"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
@@ -5339,10 +5339,10 @@
       <c r="B44" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="83" t="s">
+      <c r="C44" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="D44" s="83"/>
+      <c r="D44" s="85"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
@@ -5379,10 +5379,10 @@
       <c r="B47" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="82" t="s">
+      <c r="C47" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="82"/>
+      <c r="D47" s="84"/>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
@@ -5391,10 +5391,10 @@
       <c r="B48" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="C48" s="83" t="s">
+      <c r="C48" s="85" t="s">
         <v>229</v>
       </c>
-      <c r="D48" s="83"/>
+      <c r="D48" s="85"/>
     </row>
     <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
@@ -5403,10 +5403,10 @@
       <c r="B49" s="49" t="s">
         <v>223</v>
       </c>
-      <c r="C49" s="87" t="s">
+      <c r="C49" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="D49" s="88"/>
+      <c r="D49" s="83"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
@@ -5443,10 +5443,10 @@
       <c r="B52" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="82" t="s">
+      <c r="C52" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D52" s="82"/>
+      <c r="D52" s="84"/>
     </row>
     <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
@@ -5455,10 +5455,10 @@
       <c r="B53" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="C53" s="83" t="s">
+      <c r="C53" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="D53" s="83"/>
+      <c r="D53" s="85"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
@@ -5495,10 +5495,10 @@
       <c r="B56" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="82" t="s">
+      <c r="C56" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D56" s="82"/>
+      <c r="D56" s="84"/>
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
@@ -5507,13 +5507,29 @@
       <c r="B57" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="83" t="s">
+      <c r="C57" s="85" t="s">
         <v>177</v>
       </c>
-      <c r="D57" s="83"/>
+      <c r="D57" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C11:D11"/>
@@ -5530,22 +5546,6 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5569,15 +5569,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6022,6 +6022,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C10CBD0BFFFC4C45AC3F11163104E16D" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="262411e6662ad09615282c69781eb9d9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b60a26d6-954b-4ea8-8ffb-45e6dc51f000" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c47ce3659eb4404f7d05dc3dfe6d55d0" ns2:_="">
     <xsd:import namespace="b60a26d6-954b-4ea8-8ffb-45e6dc51f000"/>
@@ -6153,22 +6168,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F3655E-FF67-4DBD-8937-399569529388}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BB517A3-CC67-477D-B6B3-FBDAE4AB9BBA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF39737-84FF-4EF8-BD97-5D0EF02227DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6184,21 +6201,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BB517A3-CC67-477D-B6B3-FBDAE4AB9BBA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F3655E-FF67-4DBD-8937-399569529388}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>